<commit_message>
Removed macro ini file instead of wrinting macro to the target file.
</commit_message>
<xml_diff>
--- a/starterkit/win-bat/__PREFIX__Control.xlsx
+++ b/starterkit/win-bat/__PREFIX__Control.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF2AAD-E35B-4FAA-94D1-210432798E15}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEAE20F-5567-4DD5-B12A-18DEB138581C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>state</t>
     <phoneticPr fontId="2"/>
@@ -94,6 +94,14 @@
   </si>
   <si>
     <t>brcond</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>basestate</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>exit</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -617,13 +625,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="18.75"/>
@@ -683,80 +691,91 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:5" s="7" customFormat="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" s="11" customFormat="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" ht="18.75" customHeight="1">
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" s="11" customFormat="1">
       <c r="A7" s="10"/>
-      <c r="B7" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" s="11" customFormat="1" ht="18.75" customHeight="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" s="11" customFormat="1">
+      <c r="E8" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="19.5" customHeight="1">
       <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:5" s="13" customFormat="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+    <row r="10" spans="1:5" s="11" customFormat="1">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" s="13" customFormat="1">
       <c r="A11" s="12"/>
       <c r="B11" s="12" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5" s="14" customFormat="1"/>
-    <row r="13" spans="1:5" s="14" customFormat="1">
-      <c r="B13" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="12" spans="1:5" s="13" customFormat="1">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" s="14" customFormat="1"/>
     <row r="14" spans="1:5" s="14" customFormat="1">
       <c r="B14" s="14" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="14" customFormat="1">
       <c r="B15" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="14" customFormat="1">
+      <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>